<commit_message>
Fixed issue with contraindications and with completions not showing when Pneumo 65+ was finished
</commit_message>
<xml_diff>
--- a/schedules/Pneumo65.xlsx
+++ b/schedules/Pneumo65.xlsx
@@ -9,23 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="389"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$136</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$L$136</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$140</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$L$140</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="66">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -208,6 +207,21 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>8 weeks</t>
+  </si>
+  <si>
+    <t>1 y -8 w -4 d</t>
+  </si>
+  <si>
+    <t>In case of contraindicated dose</t>
+  </si>
+  <si>
+    <t>Interval After</t>
+  </si>
+  <si>
+    <t>5 years</t>
   </si>
 </sst>
 </file>
@@ -248,7 +262,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +303,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
         <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="26"/>
       </patternFill>
     </fill>
   </fills>
@@ -369,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -435,6 +455,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -497,19 +520,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>358357</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>141164</xdr:rowOff>
+      <xdr:colOff>910807</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>131639</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -528,7 +551,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="390525" y="3257550"/>
+          <a:off x="942975" y="3086100"/>
           <a:ext cx="6435307" cy="5732339"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -889,12 +912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K135"/>
+  <dimension ref="B1:K139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -923,13 +945,13 @@
       <c r="D2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
@@ -1017,11 +1039,11 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
@@ -1071,12 +1093,12 @@
       <c r="F60" s="14"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B61" s="28" t="s">
+      <c r="B61" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
       <c r="F61" s="14"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
@@ -1179,11 +1201,11 @@
       <c r="F70" s="14"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
       <c r="F71" s="14"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
@@ -1199,14 +1221,14 @@
       <c r="E72" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F72" s="29" t="s">
+      <c r="F72" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G72" s="30"/>
-      <c r="H72" s="30"/>
-      <c r="I72" s="30"/>
-      <c r="J72" s="30"/>
-      <c r="K72" s="31"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="31"/>
+      <c r="J72" s="31"/>
+      <c r="K72" s="32"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="9" t="s">
@@ -1219,28 +1241,28 @@
         <v>55</v>
       </c>
       <c r="E73" s="9"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="33"/>
-      <c r="H73" s="33"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="34"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="34"/>
+      <c r="H73" s="34"/>
+      <c r="I73" s="34"/>
+      <c r="J73" s="34"/>
+      <c r="K73" s="35"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="36"/>
-      <c r="J74" s="36"/>
-      <c r="K74" s="37"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="38"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" s="9" t="s">
@@ -1251,12 +1273,12 @@
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="36"/>
-      <c r="I75" s="36"/>
-      <c r="J75" s="36"/>
-      <c r="K75" s="37"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="38"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" s="17" t="s">
@@ -1298,12 +1320,12 @@
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B81" s="28" t="s">
+      <c r="B81" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="16"/>
@@ -1324,7 +1346,9 @@
       <c r="C83" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D83" s="9"/>
+      <c r="D83" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="E83" s="9" t="s">
         <v>19</v>
       </c>
@@ -1351,7 +1375,9 @@
       <c r="B86" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C86" s="9"/>
+      <c r="C86" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="D86" s="9" t="s">
         <v>51</v>
       </c>
@@ -1404,523 +1430,559 @@
       <c r="E91" s="14"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
+      <c r="B92" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F93" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G93" s="30"/>
-      <c r="H93" s="30"/>
-      <c r="I93" s="30"/>
-      <c r="J93" s="30"/>
-      <c r="K93" s="31"/>
+      <c r="F93" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="9" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="33"/>
-      <c r="H94" s="33"/>
-      <c r="I94" s="33"/>
-      <c r="J94" s="33"/>
-      <c r="K94" s="34"/>
+      <c r="F94" s="9"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B95" s="9" t="s">
+      <c r="B95" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B96" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G96" s="31"/>
+      <c r="H96" s="31"/>
+      <c r="I96" s="31"/>
+      <c r="J96" s="31"/>
+      <c r="K96" s="32"/>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B97" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="33"/>
+      <c r="G97" s="34"/>
+      <c r="H97" s="34"/>
+      <c r="I97" s="34"/>
+      <c r="J97" s="34"/>
+      <c r="K97" s="35"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B98" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C98" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D95" s="9"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="35"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="36"/>
-      <c r="I95" s="36"/>
-      <c r="J95" s="36"/>
-      <c r="K95" s="37"/>
-    </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B96" s="17" t="s">
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="36"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="37"/>
+      <c r="K98" s="38"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B99" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C99" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B97" s="17" t="s">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B100" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C100" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B98" s="5" t="s">
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B102" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C102" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14" t="s">
+      <c r="D102" s="14"/>
+      <c r="E102" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B99" s="15" t="s">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B103" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C99" s="15">
+      <c r="C103" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B100" s="28" t="s">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B104" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B101" s="16"/>
-      <c r="C101" s="6" t="s">
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" s="16"/>
+      <c r="C105" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="D105" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E101" s="6" t="s">
+      <c r="E105" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F101" s="6" t="s">
+      <c r="F105" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B102" s="17" t="s">
+    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B106" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C106" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D102" s="9" t="s">
+      <c r="D106" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E102" s="9" t="s">
+      <c r="E106" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F102" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B103" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B104" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B105" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9"/>
-    </row>
-    <row r="106" spans="2:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D106" s="9"/>
-      <c r="E106" s="9"/>
+      <c r="F106" s="28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B107" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C107" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="C107" s="9"/>
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B108" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C108" s="18"/>
+        <v>21</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B109" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+    </row>
+    <row r="110" spans="2:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" s="18"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B112" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C112" s="18"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B113" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C113" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B110" s="28" t="s">
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B114" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-    </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" s="6" t="s">
+      <c r="C114" s="29"/>
+      <c r="D114" s="29"/>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B115" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C115" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D111" s="6" t="s">
+      <c r="D115" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E111" s="6" t="s">
+      <c r="E115" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F111" s="29" t="s">
+      <c r="F115" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G111" s="30"/>
-      <c r="H111" s="30"/>
-      <c r="I111" s="30"/>
-      <c r="J111" s="30"/>
-      <c r="K111" s="31"/>
-    </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B112" s="9" t="s">
+      <c r="G115" s="31"/>
+      <c r="H115" s="31"/>
+      <c r="I115" s="31"/>
+      <c r="J115" s="31"/>
+      <c r="K115" s="32"/>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B116" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C112" s="9" t="s">
+      <c r="C116" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D112" s="9" t="s">
+      <c r="D116" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E112" s="9"/>
-      <c r="F112" s="32"/>
-      <c r="G112" s="33"/>
-      <c r="H112" s="33"/>
-      <c r="I112" s="33"/>
-      <c r="J112" s="33"/>
-      <c r="K112" s="34"/>
-    </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B113" s="9" t="s">
+      <c r="E116" s="9"/>
+      <c r="F116" s="33"/>
+      <c r="G116" s="34"/>
+      <c r="H116" s="34"/>
+      <c r="I116" s="34"/>
+      <c r="J116" s="34"/>
+      <c r="K116" s="35"/>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B117" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C117" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D113" s="9"/>
-      <c r="E113" s="9"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="24"/>
-      <c r="H113" s="24"/>
-      <c r="I113" s="24"/>
-      <c r="J113" s="24"/>
-      <c r="K113" s="25"/>
-    </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B114" s="9" t="s">
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="23"/>
+      <c r="G117" s="24"/>
+      <c r="H117" s="24"/>
+      <c r="I117" s="24"/>
+      <c r="J117" s="24"/>
+      <c r="K117" s="25"/>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B118" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C114" s="22" t="s">
+      <c r="C118" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D114" s="22"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="38"/>
-      <c r="G114" s="39"/>
-      <c r="H114" s="39"/>
-      <c r="I114" s="39"/>
-      <c r="J114" s="39"/>
-      <c r="K114" s="40"/>
-    </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B115" s="17" t="s">
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
+      <c r="F118" s="39"/>
+      <c r="G118" s="40"/>
+      <c r="H118" s="40"/>
+      <c r="I118" s="40"/>
+      <c r="J118" s="40"/>
+      <c r="K118" s="41"/>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B119" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C115" s="9">
+      <c r="C119" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B116" s="17" t="s">
+    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B120" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C116" s="9">
+      <c r="C120" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B118" s="5" t="s">
+    <row r="122" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B122" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C118" s="5" t="s">
+      <c r="C122" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D118" s="14"/>
-      <c r="E118" s="14" t="s">
+      <c r="D122" s="14"/>
+      <c r="E122" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B119" s="15" t="s">
+    <row r="123" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B123" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C119" s="15">
+      <c r="C123" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B120" s="28" t="s">
+    <row r="124" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B124" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="28"/>
-      <c r="D120" s="28"/>
-      <c r="E120" s="28"/>
-    </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B121" s="16"/>
-      <c r="C121" s="6" t="s">
+      <c r="C124" s="29"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="29"/>
+    </row>
+    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B125" s="16"/>
+      <c r="C125" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D121" s="6" t="s">
+      <c r="D125" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E121" s="6" t="s">
+      <c r="E125" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F121" s="6" t="s">
+      <c r="F125" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B122" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C122" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F122" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="123" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B123" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C123" s="9"/>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9"/>
-    </row>
-    <row r="124" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B124" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C124" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D124" s="9"/>
-      <c r="E124" s="9"/>
-    </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B125" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C125" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D125" s="9"/>
-      <c r="E125" s="9"/>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B126" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D126" s="9"/>
-      <c r="E126" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="D126" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F126" s="28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B127" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C127" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="C127" s="9"/>
       <c r="D127" s="9"/>
       <c r="E127" s="9"/>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B128" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C128" s="18"/>
+        <v>21</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="D128" s="9"/>
       <c r="E128" s="9"/>
     </row>
     <row r="129" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B129" s="17" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D129" s="14"/>
-      <c r="E129" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
     </row>
     <row r="130" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B130" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C130" s="28"/>
-      <c r="D130" s="28"/>
+      <c r="B130" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
     </row>
     <row r="131" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B131" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E131" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F131" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G131" s="30"/>
-      <c r="H131" s="30"/>
-      <c r="I131" s="30"/>
-      <c r="J131" s="30"/>
-      <c r="K131" s="31"/>
+      <c r="B131" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C131" s="18"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B132" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C132" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="B132" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C132" s="18"/>
       <c r="D132" s="9"/>
       <c r="E132" s="9"/>
-      <c r="F132" s="32"/>
-      <c r="G132" s="33"/>
-      <c r="H132" s="33"/>
-      <c r="I132" s="33"/>
-      <c r="J132" s="33"/>
-      <c r="K132" s="34"/>
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B133" s="9" t="s">
+      <c r="B133" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C133" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C133" s="9" t="s">
+      <c r="D133" s="14"/>
+      <c r="E133" s="14"/>
+    </row>
+    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B134" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C134" s="29"/>
+      <c r="D134" s="29"/>
+    </row>
+    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B135" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F135" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G135" s="31"/>
+      <c r="H135" s="31"/>
+      <c r="I135" s="31"/>
+      <c r="J135" s="31"/>
+      <c r="K135" s="32"/>
+    </row>
+    <row r="136" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B136" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="33"/>
+      <c r="G136" s="34"/>
+      <c r="H136" s="34"/>
+      <c r="I136" s="34"/>
+      <c r="J136" s="34"/>
+      <c r="K136" s="35"/>
+    </row>
+    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B137" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D133" s="9"/>
-      <c r="E133" s="9"/>
-      <c r="F133" s="32"/>
-      <c r="G133" s="33"/>
-      <c r="H133" s="33"/>
-      <c r="I133" s="33"/>
-      <c r="J133" s="33"/>
-      <c r="K133" s="34"/>
-    </row>
-    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B134" s="17" t="s">
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="33"/>
+      <c r="G137" s="34"/>
+      <c r="H137" s="34"/>
+      <c r="I137" s="34"/>
+      <c r="J137" s="34"/>
+      <c r="K137" s="35"/>
+    </row>
+    <row r="138" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B138" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C134" s="9">
+      <c r="C138" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B135" s="17" t="s">
+    <row r="139" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B139" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C135" s="9">
+      <c r="C139" s="9">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="23">
-    <mergeCell ref="F93:K93"/>
-    <mergeCell ref="F94:K94"/>
-    <mergeCell ref="F111:K111"/>
-    <mergeCell ref="F112:K112"/>
-    <mergeCell ref="F131:K131"/>
-    <mergeCell ref="F95:K95"/>
-    <mergeCell ref="F114:K114"/>
-    <mergeCell ref="F133:K133"/>
-    <mergeCell ref="B120:E120"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B100:E100"/>
-    <mergeCell ref="F132:K132"/>
+  <mergeCells count="24">
+    <mergeCell ref="F96:K96"/>
+    <mergeCell ref="F97:K97"/>
+    <mergeCell ref="F115:K115"/>
+    <mergeCell ref="F116:K116"/>
+    <mergeCell ref="F135:K135"/>
+    <mergeCell ref="F98:K98"/>
+    <mergeCell ref="F118:K118"/>
+    <mergeCell ref="F137:K137"/>
+    <mergeCell ref="B124:E124"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B134:D134"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="F136:K136"/>
+    <mergeCell ref="B92:D92"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="B61:E61"/>
     <mergeCell ref="B81:E81"/>
     <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B95:D95"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="F72:K72"/>
     <mergeCell ref="F73:K73"/>
@@ -1934,10 +1996,11 @@
     <oddHeader>&amp;C&amp;F</oddHeader>
     <oddFooter>&amp;CPrepared by  Nathan Bunker &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
-  <rowBreaks count="3" manualBreakCount="3">
+  <rowBreaks count="4" manualBreakCount="4">
     <brk id="18" max="11" man="1"/>
     <brk id="57" max="16383" man="1"/>
-    <brk id="97" max="11" man="1"/>
+    <brk id="78" max="11" man="1"/>
+    <brk id="101" max="11" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -1945,13 +2008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A60"/>
+  <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="1">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2053,7 +2113,7 @@
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B74&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C74&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D74&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F74&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C1" age="" reason="" historyOfVaccineName=""/&gt;</v>
+        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C2" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -2076,14 +2136,14 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;" intervalGrace="&amp;CHAR(34)&amp;Schedules!F83&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="65 years" interval="" grace="4 days" intervalGrace=""/&gt;</v>
+        <v xml:space="preserve">    &lt;valid age="65 years" interval="8 weeks" grace="4 days" intervalGrace=""/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
@@ -2101,7 +2161,7 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;overdue age="" interval="13 months" grace=""/&gt;</v>
+        <v xml:space="preserve">    &lt;overdue age="66 years" interval="13 months" grace=""/&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
@@ -2135,187 +2195,193 @@
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="PCV13" schedule="INVALID" age="" reason="" historyOfVaccineName=""/&gt;</v>
+      <c r="A30" s="20" t="str">
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;contraindicate vaccineName="PPSV" afterInterval="5 years" age="" reason="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B97&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D97&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F97&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E97&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="PCV13" schedule="INVALID" age="" reason="" historyOfVaccineName=""/&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F98&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="COMPLETE" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="str">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B99&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D99&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="C1" dose="1" indication="" label="PCV-13 after PPSV"&gt;</v>
-      </c>
-    </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;pos row="2" column="1"/&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B103&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="C1" dose="1" indication="" label="PCV-13 after PPSV"&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D102&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;" intervalGrace="&amp;CHAR(34)&amp;Schedules!F102&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="65 years" interval="1 year" grace="46 years" intervalGrace="4 days"/&gt;</v>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C120&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;pos row="2" column="1"/&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;" intervalGrace="&amp;CHAR(34)&amp;Schedules!F106&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;valid age="65 years" interval="1 year" grace="46 years" intervalGrace="1 y -8 w -4 d"/&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;due age="65 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;overdue age="66 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;due age="65 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="120 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;overdue age="66 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E110&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;finished age="120 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D111&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E111&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="str">
-        <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="20" t="str">
+        <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="PCV13"/&gt;</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B112&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C112&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F112&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C1" age="65 years -4 days" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B113&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F113&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C2" age="" reason="" historyOfVaccineName=""/&gt;</v>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C1" age="65 years -4 days" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B114&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D114&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F114&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E114&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B117&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D117&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F117&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E117&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C2" age="" reason="" historyOfVaccineName=""/&gt;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B118&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D118&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F118&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E118&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV13" schedule="S1" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="str">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B119&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D119&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E118&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="C2" dose="1" indication="" label="PCV-13 after PPSVs"&gt;</v>
-      </c>
-    </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B123&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C123&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E122&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="C2" dose="1" indication="" label="PCV-13 after PPSVs"&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C122&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D122&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E122&amp;CHAR(34)&amp;" intervalGrace="&amp;CHAR(34)&amp;Schedules!F122&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="65 years" interval="1 year" grace="46 years" intervalGrace="4 days"/&gt;</v>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C139&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C138&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C123&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E123&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C126&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E126&amp;CHAR(34)&amp;" intervalGrace="&amp;CHAR(34)&amp;Schedules!F126&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;valid age="65 years" interval="1 year" grace="46 years" intervalGrace="1 y -8 w -4 d"/&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C124&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E124&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;due age="65 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C127&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E127&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C125&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E125&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;overdue age="66 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C128&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E128&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;due age="65 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C126&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E126&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="120 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C129&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E129&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;overdue age="66 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E127&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C130&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E130&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;finished age="120 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D131&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E131&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="str">
-        <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C129&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="20" t="str">
+        <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="PCV13"/&gt;</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B132&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F132&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C2" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B133&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F133&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B136&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F136&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="PPSV" schedule="C2" age="" reason="" historyOfVaccineName=""/&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B137&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F137&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV13" schedule="COMPLETE" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="20" t="str">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="19" t="str">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="19" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>
       </c>

</xml_diff>